<commit_message>
5 numaralı formda renkli kutucuk düzenlemesi
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/05_Cellguide Peene_II_III.xlsx
+++ b/WebApplication1/Forms/05_Cellguide Peene_II_III.xlsx
@@ -212,7 +212,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="166" formatCode="[Blue][=1]0;[Red][=2]0;0;"/>
+    <numFmt numFmtId="166" formatCode="[Blue][=1]\█;[Red][=2]\█;0;"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -996,6 +996,9 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1007,9 +1010,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1056,9 +1056,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="23" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1091,6 +1088,9 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="166" fontId="23" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1109,80 +1109,7 @@
     <cellStyle name="Normal - Style1" xfId="9"/>
     <cellStyle name="Total" xfId="10" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="39"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="39"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="39"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="39"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="39"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="39"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1885,7 +1812,7 @@
   <dimension ref="A1:BK164"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="BN8" sqref="BN8"/>
+      <selection activeCell="T3" sqref="T3:U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1919,31 +1846,31 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="4"/>
-      <c r="P1" s="115">
+      <c r="P1" s="123">
         <v>1</v>
       </c>
-      <c r="Q1" s="115"/>
+      <c r="Q1" s="123"/>
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
-      <c r="U1" s="115">
+      <c r="U1" s="123">
         <v>2</v>
       </c>
-      <c r="V1" s="115"/>
+      <c r="V1" s="123"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
-      <c r="Z1" s="115">
+      <c r="Z1" s="123">
         <v>3</v>
       </c>
-      <c r="AA1" s="115"/>
+      <c r="AA1" s="123"/>
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
-      <c r="AE1" s="115">
+      <c r="AE1" s="123">
         <v>4</v>
       </c>
-      <c r="AF1" s="115"/>
+      <c r="AF1" s="123"/>
       <c r="AG1" s="4"/>
       <c r="AH1" s="4"/>
       <c r="AI1" s="4"/>
@@ -2059,32 +1986,30 @@
       <c r="M3" s="17"/>
       <c r="N3" s="15"/>
       <c r="O3" s="18"/>
-      <c r="P3" s="116">
+      <c r="P3" s="115">
         <v>1</v>
       </c>
-      <c r="Q3" s="117"/>
+      <c r="Q3" s="116"/>
       <c r="R3" s="9"/>
       <c r="S3" s="9"/>
-      <c r="T3" s="117">
-        <v>2</v>
-      </c>
-      <c r="U3" s="120"/>
-      <c r="V3" s="116"/>
-      <c r="W3" s="117"/>
+      <c r="T3" s="116"/>
+      <c r="U3" s="119"/>
+      <c r="V3" s="115"/>
+      <c r="W3" s="116"/>
       <c r="X3" s="9"/>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="120"/>
-      <c r="AA3" s="116"/>
-      <c r="AB3" s="117"/>
+      <c r="Y3" s="116"/>
+      <c r="Z3" s="119"/>
+      <c r="AA3" s="115"/>
+      <c r="AB3" s="116"/>
       <c r="AC3" s="9"/>
-      <c r="AD3" s="117"/>
-      <c r="AE3" s="120"/>
-      <c r="AF3" s="116"/>
-      <c r="AG3" s="117"/>
+      <c r="AD3" s="116"/>
+      <c r="AE3" s="119"/>
+      <c r="AF3" s="115"/>
+      <c r="AG3" s="116"/>
       <c r="AH3" s="9"/>
       <c r="AI3" s="9"/>
-      <c r="AJ3" s="117"/>
-      <c r="AK3" s="120"/>
+      <c r="AJ3" s="116"/>
+      <c r="AK3" s="119"/>
       <c r="AL3" s="19"/>
       <c r="AM3" s="9"/>
       <c r="AN3" s="9"/>
@@ -2134,28 +2059,28 @@
       <c r="M4" s="17"/>
       <c r="N4" s="15"/>
       <c r="O4" s="18"/>
-      <c r="P4" s="118"/>
-      <c r="Q4" s="119"/>
+      <c r="P4" s="117"/>
+      <c r="Q4" s="118"/>
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="119"/>
-      <c r="U4" s="121"/>
-      <c r="V4" s="118"/>
-      <c r="W4" s="119"/>
+      <c r="T4" s="118"/>
+      <c r="U4" s="120"/>
+      <c r="V4" s="117"/>
+      <c r="W4" s="118"/>
       <c r="X4" s="9"/>
-      <c r="Y4" s="119"/>
-      <c r="Z4" s="121"/>
-      <c r="AA4" s="118"/>
-      <c r="AB4" s="119"/>
+      <c r="Y4" s="118"/>
+      <c r="Z4" s="120"/>
+      <c r="AA4" s="117"/>
+      <c r="AB4" s="118"/>
       <c r="AC4" s="9"/>
-      <c r="AD4" s="119"/>
-      <c r="AE4" s="121"/>
-      <c r="AF4" s="118"/>
-      <c r="AG4" s="119"/>
+      <c r="AD4" s="118"/>
+      <c r="AE4" s="120"/>
+      <c r="AF4" s="117"/>
+      <c r="AG4" s="118"/>
       <c r="AH4" s="9"/>
       <c r="AI4" s="9"/>
-      <c r="AJ4" s="119"/>
-      <c r="AK4" s="121"/>
+      <c r="AJ4" s="118"/>
+      <c r="AK4" s="120"/>
       <c r="AL4" s="21"/>
       <c r="AM4" s="9"/>
       <c r="AN4" s="9"/>
@@ -2530,28 +2455,30 @@
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
       <c r="O10" s="18"/>
-      <c r="P10" s="118"/>
-      <c r="Q10" s="119"/>
+      <c r="P10" s="117">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="118"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
-      <c r="T10" s="119"/>
-      <c r="U10" s="121"/>
-      <c r="V10" s="118"/>
-      <c r="W10" s="119"/>
+      <c r="T10" s="118"/>
+      <c r="U10" s="120"/>
+      <c r="V10" s="117"/>
+      <c r="W10" s="118"/>
       <c r="X10" s="9"/>
-      <c r="Y10" s="119"/>
-      <c r="Z10" s="121"/>
-      <c r="AA10" s="118"/>
-      <c r="AB10" s="119"/>
+      <c r="Y10" s="118"/>
+      <c r="Z10" s="120"/>
+      <c r="AA10" s="117"/>
+      <c r="AB10" s="118"/>
       <c r="AC10" s="9"/>
-      <c r="AD10" s="119"/>
-      <c r="AE10" s="121"/>
-      <c r="AF10" s="118"/>
-      <c r="AG10" s="119"/>
+      <c r="AD10" s="118"/>
+      <c r="AE10" s="120"/>
+      <c r="AF10" s="117"/>
+      <c r="AG10" s="118"/>
       <c r="AH10" s="9"/>
       <c r="AI10" s="9"/>
-      <c r="AJ10" s="119"/>
-      <c r="AK10" s="121"/>
+      <c r="AJ10" s="118"/>
+      <c r="AK10" s="120"/>
       <c r="AL10" s="21"/>
       <c r="AM10" s="9"/>
       <c r="AN10" s="9"/>
@@ -2598,27 +2525,27 @@
       <c r="N11" s="15"/>
       <c r="O11" s="18"/>
       <c r="P11" s="124"/>
-      <c r="Q11" s="122"/>
+      <c r="Q11" s="121"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="122"/>
-      <c r="U11" s="123"/>
+      <c r="T11" s="121"/>
+      <c r="U11" s="122"/>
       <c r="V11" s="124"/>
-      <c r="W11" s="122"/>
+      <c r="W11" s="121"/>
       <c r="X11" s="9"/>
-      <c r="Y11" s="122"/>
-      <c r="Z11" s="123"/>
+      <c r="Y11" s="121"/>
+      <c r="Z11" s="122"/>
       <c r="AA11" s="124"/>
-      <c r="AB11" s="122"/>
+      <c r="AB11" s="121"/>
       <c r="AC11" s="9"/>
-      <c r="AD11" s="122"/>
-      <c r="AE11" s="123"/>
+      <c r="AD11" s="121"/>
+      <c r="AE11" s="122"/>
       <c r="AF11" s="124"/>
-      <c r="AG11" s="122"/>
+      <c r="AG11" s="121"/>
       <c r="AH11" s="9"/>
       <c r="AI11" s="9"/>
-      <c r="AJ11" s="122"/>
-      <c r="AK11" s="123"/>
+      <c r="AJ11" s="121"/>
+      <c r="AK11" s="122"/>
       <c r="AL11" s="21"/>
       <c r="AM11" s="9"/>
       <c r="AN11" s="9"/>
@@ -2783,64 +2710,64 @@
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="72"/>
-      <c r="G14" s="101">
+      <c r="G14" s="98">
         <v>1</v>
       </c>
-      <c r="H14" s="101"/>
+      <c r="H14" s="98"/>
       <c r="I14" s="72"/>
       <c r="J14" s="72"/>
-      <c r="K14" s="101">
+      <c r="K14" s="98">
         <v>2</v>
       </c>
-      <c r="L14" s="101"/>
+      <c r="L14" s="98"/>
       <c r="M14" s="72"/>
       <c r="N14" s="72"/>
       <c r="O14" s="72"/>
-      <c r="P14" s="101">
+      <c r="P14" s="98">
         <v>3</v>
       </c>
-      <c r="Q14" s="101"/>
+      <c r="Q14" s="98"/>
       <c r="R14" s="72"/>
       <c r="S14" s="72"/>
       <c r="T14" s="72"/>
-      <c r="U14" s="101">
+      <c r="U14" s="98">
         <v>4</v>
       </c>
-      <c r="V14" s="101"/>
+      <c r="V14" s="98"/>
       <c r="W14" s="72"/>
       <c r="X14" s="72"/>
       <c r="Y14" s="72"/>
-      <c r="Z14" s="101">
+      <c r="Z14" s="98">
         <v>5</v>
       </c>
-      <c r="AA14" s="101"/>
+      <c r="AA14" s="98"/>
       <c r="AB14" s="72"/>
       <c r="AC14" s="72"/>
       <c r="AD14" s="72"/>
-      <c r="AE14" s="101">
+      <c r="AE14" s="98">
         <v>6</v>
       </c>
-      <c r="AF14" s="101"/>
+      <c r="AF14" s="98"/>
       <c r="AG14" s="72"/>
       <c r="AH14" s="72"/>
       <c r="AI14" s="72"/>
-      <c r="AJ14" s="101">
+      <c r="AJ14" s="98">
         <v>7</v>
       </c>
-      <c r="AK14" s="101"/>
+      <c r="AK14" s="98"/>
       <c r="AL14" s="72"/>
       <c r="AM14" s="72"/>
       <c r="AN14" s="72"/>
-      <c r="AO14" s="101">
+      <c r="AO14" s="98">
         <v>8</v>
       </c>
-      <c r="AP14" s="101"/>
+      <c r="AP14" s="98"/>
       <c r="AQ14" s="72"/>
       <c r="AR14" s="72"/>
-      <c r="AS14" s="101">
+      <c r="AS14" s="98">
         <v>9</v>
       </c>
-      <c r="AT14" s="101"/>
+      <c r="AT14" s="98"/>
       <c r="AU14" s="72"/>
       <c r="AV14" s="15"/>
       <c r="AW14" s="15"/>
@@ -2935,46 +2862,46 @@
       <c r="D16" s="17"/>
       <c r="E16" s="15"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="99"/>
+      <c r="G16" s="99"/>
+      <c r="H16" s="100"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="100"/>
-      <c r="L16" s="98"/>
-      <c r="M16" s="99"/>
+      <c r="J16" s="100"/>
+      <c r="K16" s="101"/>
+      <c r="L16" s="99"/>
+      <c r="M16" s="100"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="99"/>
-      <c r="P16" s="100"/>
-      <c r="Q16" s="98"/>
-      <c r="R16" s="99"/>
+      <c r="O16" s="100"/>
+      <c r="P16" s="101"/>
+      <c r="Q16" s="99"/>
+      <c r="R16" s="100"/>
       <c r="S16" s="9"/>
-      <c r="T16" s="99"/>
-      <c r="U16" s="100"/>
-      <c r="V16" s="98"/>
-      <c r="W16" s="99"/>
+      <c r="T16" s="100"/>
+      <c r="U16" s="101"/>
+      <c r="V16" s="99"/>
+      <c r="W16" s="100"/>
       <c r="X16" s="9"/>
-      <c r="Y16" s="99"/>
-      <c r="Z16" s="100"/>
-      <c r="AA16" s="98"/>
-      <c r="AB16" s="99"/>
+      <c r="Y16" s="100"/>
+      <c r="Z16" s="101"/>
+      <c r="AA16" s="99"/>
+      <c r="AB16" s="100"/>
       <c r="AC16" s="9"/>
-      <c r="AD16" s="99"/>
-      <c r="AE16" s="100"/>
-      <c r="AF16" s="98"/>
-      <c r="AG16" s="99"/>
+      <c r="AD16" s="100"/>
+      <c r="AE16" s="101"/>
+      <c r="AF16" s="99"/>
+      <c r="AG16" s="100"/>
       <c r="AH16" s="9"/>
-      <c r="AI16" s="99"/>
-      <c r="AJ16" s="100"/>
-      <c r="AK16" s="98"/>
-      <c r="AL16" s="99"/>
+      <c r="AI16" s="100"/>
+      <c r="AJ16" s="101"/>
+      <c r="AK16" s="99"/>
+      <c r="AL16" s="100"/>
       <c r="AM16" s="9"/>
-      <c r="AN16" s="99"/>
-      <c r="AO16" s="100"/>
-      <c r="AP16" s="98"/>
-      <c r="AQ16" s="99"/>
+      <c r="AN16" s="100"/>
+      <c r="AO16" s="101"/>
+      <c r="AP16" s="99"/>
+      <c r="AQ16" s="100"/>
       <c r="AR16" s="9"/>
-      <c r="AS16" s="99"/>
-      <c r="AT16" s="100"/>
+      <c r="AS16" s="100"/>
+      <c r="AT16" s="101"/>
       <c r="AU16" s="21"/>
       <c r="AV16" s="9"/>
       <c r="AW16" s="9"/>
@@ -3664,8 +3591,8 @@
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="99"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="100"/>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -3675,8 +3602,8 @@
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
-      <c r="R27" s="99"/>
-      <c r="S27" s="100"/>
+      <c r="R27" s="100"/>
+      <c r="S27" s="101"/>
       <c r="T27" s="9"/>
       <c r="U27" s="9"/>
       <c r="V27" s="9"/>
@@ -3691,8 +3618,8 @@
       <c r="AE27" s="9"/>
       <c r="AF27" s="9"/>
       <c r="AG27" s="9"/>
-      <c r="AH27" s="98"/>
-      <c r="AI27" s="99"/>
+      <c r="AH27" s="99"/>
+      <c r="AI27" s="100"/>
       <c r="AJ27" s="9"/>
       <c r="AK27" s="9"/>
       <c r="AL27" s="9"/>
@@ -3702,8 +3629,8 @@
       <c r="AP27" s="9"/>
       <c r="AQ27" s="9"/>
       <c r="AR27" s="9"/>
-      <c r="AS27" s="99"/>
-      <c r="AT27" s="100"/>
+      <c r="AS27" s="100"/>
+      <c r="AT27" s="101"/>
       <c r="AV27" s="9"/>
       <c r="AW27" s="9"/>
       <c r="AX27" s="9"/>
@@ -4051,64 +3978,64 @@
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="72"/>
-      <c r="G33" s="101">
+      <c r="G33" s="98">
         <v>1</v>
       </c>
-      <c r="H33" s="101"/>
+      <c r="H33" s="98"/>
       <c r="I33" s="72"/>
       <c r="J33" s="72"/>
-      <c r="K33" s="101">
+      <c r="K33" s="98">
         <v>2</v>
       </c>
-      <c r="L33" s="101"/>
+      <c r="L33" s="98"/>
       <c r="M33" s="72"/>
       <c r="N33" s="72"/>
       <c r="O33" s="72"/>
-      <c r="P33" s="101">
+      <c r="P33" s="98">
         <v>3</v>
       </c>
-      <c r="Q33" s="101"/>
+      <c r="Q33" s="98"/>
       <c r="R33" s="72"/>
       <c r="S33" s="72"/>
       <c r="T33" s="72"/>
-      <c r="U33" s="101">
+      <c r="U33" s="98">
         <v>4</v>
       </c>
-      <c r="V33" s="101"/>
+      <c r="V33" s="98"/>
       <c r="W33" s="72"/>
       <c r="X33" s="72"/>
       <c r="Y33" s="72"/>
-      <c r="Z33" s="101">
+      <c r="Z33" s="98">
         <v>5</v>
       </c>
-      <c r="AA33" s="101"/>
+      <c r="AA33" s="98"/>
       <c r="AB33" s="72"/>
       <c r="AC33" s="72"/>
       <c r="AD33" s="72"/>
-      <c r="AE33" s="101">
+      <c r="AE33" s="98">
         <v>6</v>
       </c>
-      <c r="AF33" s="101"/>
+      <c r="AF33" s="98"/>
       <c r="AG33" s="72"/>
       <c r="AH33" s="72"/>
       <c r="AI33" s="72"/>
-      <c r="AJ33" s="101">
+      <c r="AJ33" s="98">
         <v>7</v>
       </c>
-      <c r="AK33" s="101"/>
+      <c r="AK33" s="98"/>
       <c r="AL33" s="72"/>
       <c r="AM33" s="72"/>
       <c r="AN33" s="72"/>
-      <c r="AO33" s="101">
+      <c r="AO33" s="98">
         <v>8</v>
       </c>
-      <c r="AP33" s="101"/>
+      <c r="AP33" s="98"/>
       <c r="AQ33" s="72"/>
       <c r="AR33" s="72"/>
-      <c r="AS33" s="101">
+      <c r="AS33" s="98">
         <v>9</v>
       </c>
-      <c r="AT33" s="101"/>
+      <c r="AT33" s="98"/>
       <c r="AU33" s="72"/>
       <c r="AV33" s="15"/>
       <c r="AW33" s="15"/>
@@ -4203,46 +4130,46 @@
       <c r="D35" s="17"/>
       <c r="E35" s="15"/>
       <c r="F35" s="18"/>
-      <c r="G35" s="98"/>
-      <c r="H35" s="99"/>
+      <c r="G35" s="99"/>
+      <c r="H35" s="100"/>
       <c r="I35" s="9"/>
-      <c r="J35" s="99"/>
-      <c r="K35" s="100"/>
-      <c r="L35" s="98"/>
-      <c r="M35" s="99"/>
+      <c r="J35" s="100"/>
+      <c r="K35" s="101"/>
+      <c r="L35" s="99"/>
+      <c r="M35" s="100"/>
       <c r="N35" s="9"/>
-      <c r="O35" s="99"/>
-      <c r="P35" s="100"/>
-      <c r="Q35" s="98"/>
-      <c r="R35" s="99"/>
+      <c r="O35" s="100"/>
+      <c r="P35" s="101"/>
+      <c r="Q35" s="99"/>
+      <c r="R35" s="100"/>
       <c r="S35" s="9"/>
-      <c r="T35" s="99"/>
-      <c r="U35" s="100"/>
-      <c r="V35" s="98"/>
-      <c r="W35" s="99"/>
+      <c r="T35" s="100"/>
+      <c r="U35" s="101"/>
+      <c r="V35" s="99"/>
+      <c r="W35" s="100"/>
       <c r="X35" s="9"/>
-      <c r="Y35" s="99"/>
-      <c r="Z35" s="100"/>
-      <c r="AA35" s="98"/>
-      <c r="AB35" s="99"/>
+      <c r="Y35" s="100"/>
+      <c r="Z35" s="101"/>
+      <c r="AA35" s="99"/>
+      <c r="AB35" s="100"/>
       <c r="AC35" s="9"/>
-      <c r="AD35" s="99"/>
-      <c r="AE35" s="100"/>
-      <c r="AF35" s="98"/>
-      <c r="AG35" s="99"/>
+      <c r="AD35" s="100"/>
+      <c r="AE35" s="101"/>
+      <c r="AF35" s="99"/>
+      <c r="AG35" s="100"/>
       <c r="AH35" s="9"/>
-      <c r="AI35" s="99"/>
-      <c r="AJ35" s="100"/>
-      <c r="AK35" s="98"/>
-      <c r="AL35" s="99"/>
+      <c r="AI35" s="100"/>
+      <c r="AJ35" s="101"/>
+      <c r="AK35" s="99"/>
+      <c r="AL35" s="100"/>
       <c r="AM35" s="9"/>
-      <c r="AN35" s="99"/>
-      <c r="AO35" s="100"/>
-      <c r="AP35" s="98"/>
-      <c r="AQ35" s="99"/>
+      <c r="AN35" s="100"/>
+      <c r="AO35" s="101"/>
+      <c r="AP35" s="99"/>
+      <c r="AQ35" s="100"/>
       <c r="AR35" s="9"/>
-      <c r="AS35" s="99"/>
-      <c r="AT35" s="100"/>
+      <c r="AS35" s="100"/>
+      <c r="AT35" s="101"/>
       <c r="AU35" s="21"/>
       <c r="AV35" s="9"/>
       <c r="AW35" s="9"/>
@@ -4932,64 +4859,64 @@
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
       <c r="F46" s="72"/>
-      <c r="G46" s="101">
+      <c r="G46" s="98">
         <v>1</v>
       </c>
-      <c r="H46" s="101"/>
+      <c r="H46" s="98"/>
       <c r="I46" s="72"/>
       <c r="J46" s="72"/>
-      <c r="K46" s="101">
+      <c r="K46" s="98">
         <v>2</v>
       </c>
-      <c r="L46" s="101"/>
+      <c r="L46" s="98"/>
       <c r="M46" s="72"/>
       <c r="N46" s="72"/>
       <c r="O46" s="72"/>
-      <c r="P46" s="101">
+      <c r="P46" s="98">
         <v>3</v>
       </c>
-      <c r="Q46" s="101"/>
+      <c r="Q46" s="98"/>
       <c r="R46" s="72"/>
       <c r="S46" s="72"/>
       <c r="T46" s="72"/>
-      <c r="U46" s="101">
+      <c r="U46" s="98">
         <v>4</v>
       </c>
-      <c r="V46" s="101"/>
+      <c r="V46" s="98"/>
       <c r="W46" s="72"/>
       <c r="X46" s="72"/>
       <c r="Y46" s="72"/>
-      <c r="Z46" s="101">
+      <c r="Z46" s="98">
         <v>5</v>
       </c>
-      <c r="AA46" s="101"/>
+      <c r="AA46" s="98"/>
       <c r="AB46" s="72"/>
       <c r="AC46" s="72"/>
       <c r="AD46" s="72"/>
-      <c r="AE46" s="101">
+      <c r="AE46" s="98">
         <v>6</v>
       </c>
-      <c r="AF46" s="101"/>
+      <c r="AF46" s="98"/>
       <c r="AG46" s="72"/>
       <c r="AH46" s="72"/>
       <c r="AI46" s="72"/>
-      <c r="AJ46" s="101">
+      <c r="AJ46" s="98">
         <v>7</v>
       </c>
-      <c r="AK46" s="101"/>
+      <c r="AK46" s="98"/>
       <c r="AL46" s="72"/>
       <c r="AM46" s="72"/>
       <c r="AN46" s="72"/>
-      <c r="AO46" s="101">
+      <c r="AO46" s="98">
         <v>8</v>
       </c>
-      <c r="AP46" s="101"/>
+      <c r="AP46" s="98"/>
       <c r="AQ46" s="72"/>
       <c r="AR46" s="72"/>
-      <c r="AS46" s="101">
+      <c r="AS46" s="98">
         <v>9</v>
       </c>
-      <c r="AT46" s="101"/>
+      <c r="AT46" s="98"/>
       <c r="AU46" s="72"/>
       <c r="AV46" s="15"/>
       <c r="AW46" s="15"/>
@@ -5084,46 +5011,46 @@
       <c r="D48" s="17"/>
       <c r="E48" s="15"/>
       <c r="F48" s="18"/>
-      <c r="G48" s="98"/>
-      <c r="H48" s="99"/>
+      <c r="G48" s="99"/>
+      <c r="H48" s="100"/>
       <c r="I48" s="9"/>
-      <c r="J48" s="99"/>
-      <c r="K48" s="100"/>
-      <c r="L48" s="98"/>
-      <c r="M48" s="99"/>
+      <c r="J48" s="100"/>
+      <c r="K48" s="101"/>
+      <c r="L48" s="99"/>
+      <c r="M48" s="100"/>
       <c r="N48" s="9"/>
-      <c r="O48" s="99"/>
-      <c r="P48" s="100"/>
-      <c r="Q48" s="98"/>
-      <c r="R48" s="99"/>
+      <c r="O48" s="100"/>
+      <c r="P48" s="101"/>
+      <c r="Q48" s="99"/>
+      <c r="R48" s="100"/>
       <c r="S48" s="9"/>
-      <c r="T48" s="99"/>
-      <c r="U48" s="100"/>
-      <c r="V48" s="98"/>
-      <c r="W48" s="99"/>
+      <c r="T48" s="100"/>
+      <c r="U48" s="101"/>
+      <c r="V48" s="99"/>
+      <c r="W48" s="100"/>
       <c r="X48" s="9"/>
-      <c r="Y48" s="99"/>
-      <c r="Z48" s="100"/>
-      <c r="AA48" s="98"/>
-      <c r="AB48" s="99"/>
+      <c r="Y48" s="100"/>
+      <c r="Z48" s="101"/>
+      <c r="AA48" s="99"/>
+      <c r="AB48" s="100"/>
       <c r="AC48" s="9"/>
-      <c r="AD48" s="99"/>
-      <c r="AE48" s="100"/>
-      <c r="AF48" s="98"/>
-      <c r="AG48" s="99"/>
+      <c r="AD48" s="100"/>
+      <c r="AE48" s="101"/>
+      <c r="AF48" s="99"/>
+      <c r="AG48" s="100"/>
       <c r="AH48" s="9"/>
-      <c r="AI48" s="99"/>
-      <c r="AJ48" s="100"/>
-      <c r="AK48" s="98"/>
-      <c r="AL48" s="99"/>
+      <c r="AI48" s="100"/>
+      <c r="AJ48" s="101"/>
+      <c r="AK48" s="99"/>
+      <c r="AL48" s="100"/>
       <c r="AM48" s="9"/>
-      <c r="AN48" s="99"/>
-      <c r="AO48" s="100"/>
-      <c r="AP48" s="98"/>
-      <c r="AQ48" s="99"/>
+      <c r="AN48" s="100"/>
+      <c r="AO48" s="101"/>
+      <c r="AP48" s="99"/>
+      <c r="AQ48" s="100"/>
       <c r="AR48" s="9"/>
-      <c r="AS48" s="99"/>
-      <c r="AT48" s="100"/>
+      <c r="AS48" s="100"/>
+      <c r="AT48" s="101"/>
       <c r="AU48" s="21"/>
       <c r="AV48" s="9"/>
       <c r="AW48" s="9"/>
@@ -5813,8 +5740,8 @@
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
       <c r="F59" s="9"/>
-      <c r="G59" s="98"/>
-      <c r="H59" s="99"/>
+      <c r="G59" s="99"/>
+      <c r="H59" s="100"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
@@ -5824,8 +5751,8 @@
       <c r="O59" s="9"/>
       <c r="P59" s="9"/>
       <c r="Q59" s="9"/>
-      <c r="R59" s="99"/>
-      <c r="S59" s="100"/>
+      <c r="R59" s="100"/>
+      <c r="S59" s="101"/>
       <c r="T59" s="9"/>
       <c r="U59" s="9"/>
       <c r="V59" s="9"/>
@@ -5840,8 +5767,8 @@
       <c r="AE59" s="9"/>
       <c r="AF59" s="9"/>
       <c r="AG59" s="9"/>
-      <c r="AH59" s="98"/>
-      <c r="AI59" s="99"/>
+      <c r="AH59" s="99"/>
+      <c r="AI59" s="100"/>
       <c r="AJ59" s="9"/>
       <c r="AK59" s="9"/>
       <c r="AL59" s="9"/>
@@ -5851,8 +5778,8 @@
       <c r="AP59" s="9"/>
       <c r="AQ59" s="9"/>
       <c r="AR59" s="9"/>
-      <c r="AS59" s="99"/>
-      <c r="AT59" s="100"/>
+      <c r="AS59" s="100"/>
+      <c r="AT59" s="101"/>
       <c r="AV59" s="9"/>
       <c r="AW59" s="9"/>
       <c r="AX59" s="9"/>
@@ -6417,46 +6344,46 @@
       </c>
       <c r="E68" s="15"/>
       <c r="F68" s="18"/>
-      <c r="G68" s="98"/>
-      <c r="H68" s="99"/>
+      <c r="G68" s="99"/>
+      <c r="H68" s="100"/>
       <c r="I68" s="9"/>
-      <c r="J68" s="99"/>
-      <c r="K68" s="100"/>
-      <c r="L68" s="98"/>
-      <c r="M68" s="99"/>
+      <c r="J68" s="100"/>
+      <c r="K68" s="101"/>
+      <c r="L68" s="99"/>
+      <c r="M68" s="100"/>
       <c r="N68" s="9"/>
-      <c r="O68" s="99"/>
-      <c r="P68" s="100"/>
-      <c r="Q68" s="98"/>
-      <c r="R68" s="99"/>
+      <c r="O68" s="100"/>
+      <c r="P68" s="101"/>
+      <c r="Q68" s="99"/>
+      <c r="R68" s="100"/>
       <c r="S68" s="9"/>
-      <c r="T68" s="99"/>
-      <c r="U68" s="100"/>
-      <c r="V68" s="98"/>
-      <c r="W68" s="99"/>
+      <c r="T68" s="100"/>
+      <c r="U68" s="101"/>
+      <c r="V68" s="99"/>
+      <c r="W68" s="100"/>
       <c r="X68" s="9"/>
-      <c r="Y68" s="99"/>
-      <c r="Z68" s="100"/>
-      <c r="AA68" s="98"/>
-      <c r="AB68" s="99"/>
+      <c r="Y68" s="100"/>
+      <c r="Z68" s="101"/>
+      <c r="AA68" s="99"/>
+      <c r="AB68" s="100"/>
       <c r="AC68" s="9"/>
-      <c r="AD68" s="99"/>
-      <c r="AE68" s="100"/>
-      <c r="AF68" s="98"/>
-      <c r="AG68" s="99"/>
+      <c r="AD68" s="100"/>
+      <c r="AE68" s="101"/>
+      <c r="AF68" s="99"/>
+      <c r="AG68" s="100"/>
       <c r="AH68" s="9"/>
-      <c r="AI68" s="99"/>
-      <c r="AJ68" s="100"/>
-      <c r="AK68" s="98"/>
-      <c r="AL68" s="99"/>
+      <c r="AI68" s="100"/>
+      <c r="AJ68" s="101"/>
+      <c r="AK68" s="99"/>
+      <c r="AL68" s="100"/>
       <c r="AM68" s="9"/>
-      <c r="AN68" s="99"/>
-      <c r="AO68" s="100"/>
-      <c r="AP68" s="98"/>
-      <c r="AQ68" s="99"/>
+      <c r="AN68" s="100"/>
+      <c r="AO68" s="101"/>
+      <c r="AP68" s="99"/>
+      <c r="AQ68" s="100"/>
       <c r="AR68" s="9"/>
-      <c r="AS68" s="99"/>
-      <c r="AT68" s="100"/>
+      <c r="AS68" s="100"/>
+      <c r="AT68" s="101"/>
       <c r="AU68" s="21"/>
       <c r="AV68" s="9"/>
       <c r="AW68" s="9"/>
@@ -7146,64 +7073,64 @@
       <c r="D79" s="15"/>
       <c r="E79" s="15"/>
       <c r="F79" s="72"/>
-      <c r="G79" s="101">
+      <c r="G79" s="98">
         <v>1</v>
       </c>
-      <c r="H79" s="101"/>
+      <c r="H79" s="98"/>
       <c r="I79" s="72"/>
       <c r="J79" s="72"/>
-      <c r="K79" s="101">
+      <c r="K79" s="98">
         <v>2</v>
       </c>
-      <c r="L79" s="101"/>
+      <c r="L79" s="98"/>
       <c r="M79" s="72"/>
       <c r="N79" s="72"/>
       <c r="O79" s="72"/>
-      <c r="P79" s="101">
+      <c r="P79" s="98">
         <v>3</v>
       </c>
-      <c r="Q79" s="101"/>
+      <c r="Q79" s="98"/>
       <c r="R79" s="72"/>
       <c r="S79" s="72"/>
       <c r="T79" s="72"/>
-      <c r="U79" s="101">
+      <c r="U79" s="98">
         <v>4</v>
       </c>
-      <c r="V79" s="101"/>
+      <c r="V79" s="98"/>
       <c r="W79" s="72"/>
       <c r="X79" s="72"/>
       <c r="Y79" s="72"/>
-      <c r="Z79" s="101">
+      <c r="Z79" s="98">
         <v>5</v>
       </c>
-      <c r="AA79" s="101"/>
+      <c r="AA79" s="98"/>
       <c r="AB79" s="72"/>
       <c r="AC79" s="72"/>
       <c r="AD79" s="72"/>
-      <c r="AE79" s="101">
+      <c r="AE79" s="98">
         <v>6</v>
       </c>
-      <c r="AF79" s="101"/>
+      <c r="AF79" s="98"/>
       <c r="AG79" s="72"/>
       <c r="AH79" s="72"/>
       <c r="AI79" s="72"/>
-      <c r="AJ79" s="101">
+      <c r="AJ79" s="98">
         <v>7</v>
       </c>
-      <c r="AK79" s="101"/>
+      <c r="AK79" s="98"/>
       <c r="AL79" s="72"/>
       <c r="AM79" s="72"/>
       <c r="AN79" s="72"/>
-      <c r="AO79" s="101">
+      <c r="AO79" s="98">
         <v>8</v>
       </c>
-      <c r="AP79" s="101"/>
+      <c r="AP79" s="98"/>
       <c r="AQ79" s="72"/>
       <c r="AR79" s="72"/>
-      <c r="AS79" s="101">
+      <c r="AS79" s="98">
         <v>9</v>
       </c>
-      <c r="AT79" s="101"/>
+      <c r="AT79" s="98"/>
       <c r="AU79" s="72"/>
       <c r="AV79" s="9"/>
       <c r="AW79" s="9"/>
@@ -7298,46 +7225,46 @@
       </c>
       <c r="E81" s="15"/>
       <c r="F81" s="18"/>
-      <c r="G81" s="98"/>
-      <c r="H81" s="99"/>
+      <c r="G81" s="99"/>
+      <c r="H81" s="100"/>
       <c r="I81" s="9"/>
-      <c r="J81" s="99"/>
-      <c r="K81" s="100"/>
-      <c r="L81" s="98"/>
-      <c r="M81" s="99"/>
+      <c r="J81" s="100"/>
+      <c r="K81" s="101"/>
+      <c r="L81" s="99"/>
+      <c r="M81" s="100"/>
       <c r="N81" s="9"/>
-      <c r="O81" s="99"/>
-      <c r="P81" s="100"/>
-      <c r="Q81" s="98"/>
-      <c r="R81" s="99"/>
+      <c r="O81" s="100"/>
+      <c r="P81" s="101"/>
+      <c r="Q81" s="99"/>
+      <c r="R81" s="100"/>
       <c r="S81" s="9"/>
-      <c r="T81" s="99"/>
-      <c r="U81" s="100"/>
-      <c r="V81" s="98"/>
-      <c r="W81" s="99"/>
+      <c r="T81" s="100"/>
+      <c r="U81" s="101"/>
+      <c r="V81" s="99"/>
+      <c r="W81" s="100"/>
       <c r="X81" s="9"/>
-      <c r="Y81" s="99"/>
-      <c r="Z81" s="100"/>
-      <c r="AA81" s="98"/>
-      <c r="AB81" s="99"/>
+      <c r="Y81" s="100"/>
+      <c r="Z81" s="101"/>
+      <c r="AA81" s="99"/>
+      <c r="AB81" s="100"/>
       <c r="AC81" s="9"/>
-      <c r="AD81" s="99"/>
-      <c r="AE81" s="100"/>
-      <c r="AF81" s="98"/>
-      <c r="AG81" s="99"/>
+      <c r="AD81" s="100"/>
+      <c r="AE81" s="101"/>
+      <c r="AF81" s="99"/>
+      <c r="AG81" s="100"/>
       <c r="AH81" s="9"/>
-      <c r="AI81" s="99"/>
-      <c r="AJ81" s="100"/>
-      <c r="AK81" s="98"/>
-      <c r="AL81" s="99"/>
+      <c r="AI81" s="100"/>
+      <c r="AJ81" s="101"/>
+      <c r="AK81" s="99"/>
+      <c r="AL81" s="100"/>
       <c r="AM81" s="9"/>
-      <c r="AN81" s="99"/>
-      <c r="AO81" s="100"/>
-      <c r="AP81" s="98"/>
-      <c r="AQ81" s="99"/>
+      <c r="AN81" s="100"/>
+      <c r="AO81" s="101"/>
+      <c r="AP81" s="99"/>
+      <c r="AQ81" s="100"/>
       <c r="AR81" s="9"/>
-      <c r="AS81" s="99"/>
-      <c r="AT81" s="100"/>
+      <c r="AS81" s="100"/>
+      <c r="AT81" s="101"/>
       <c r="AU81" s="21"/>
       <c r="AV81" s="9"/>
       <c r="AW81" s="9"/>
@@ -8027,64 +7954,64 @@
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
       <c r="F92" s="72"/>
-      <c r="G92" s="101">
+      <c r="G92" s="98">
         <v>1</v>
       </c>
-      <c r="H92" s="101"/>
+      <c r="H92" s="98"/>
       <c r="I92" s="72"/>
       <c r="J92" s="72"/>
-      <c r="K92" s="101">
+      <c r="K92" s="98">
         <v>2</v>
       </c>
-      <c r="L92" s="101"/>
+      <c r="L92" s="98"/>
       <c r="M92" s="72"/>
       <c r="N92" s="72"/>
       <c r="O92" s="72"/>
-      <c r="P92" s="101">
+      <c r="P92" s="98">
         <v>3</v>
       </c>
-      <c r="Q92" s="101"/>
+      <c r="Q92" s="98"/>
       <c r="R92" s="72"/>
       <c r="S92" s="72"/>
       <c r="T92" s="72"/>
-      <c r="U92" s="101">
+      <c r="U92" s="98">
         <v>4</v>
       </c>
-      <c r="V92" s="101"/>
+      <c r="V92" s="98"/>
       <c r="W92" s="72"/>
       <c r="X92" s="72"/>
       <c r="Y92" s="72"/>
-      <c r="Z92" s="101">
+      <c r="Z92" s="98">
         <v>5</v>
       </c>
-      <c r="AA92" s="101"/>
+      <c r="AA92" s="98"/>
       <c r="AB92" s="72"/>
       <c r="AC92" s="72"/>
       <c r="AD92" s="72"/>
-      <c r="AE92" s="101">
+      <c r="AE92" s="98">
         <v>6</v>
       </c>
-      <c r="AF92" s="101"/>
+      <c r="AF92" s="98"/>
       <c r="AG92" s="72"/>
       <c r="AH92" s="72"/>
       <c r="AI92" s="72"/>
-      <c r="AJ92" s="101">
+      <c r="AJ92" s="98">
         <v>7</v>
       </c>
-      <c r="AK92" s="101"/>
+      <c r="AK92" s="98"/>
       <c r="AL92" s="72"/>
       <c r="AM92" s="72"/>
       <c r="AN92" s="72"/>
-      <c r="AO92" s="101">
+      <c r="AO92" s="98">
         <v>8</v>
       </c>
-      <c r="AP92" s="101"/>
+      <c r="AP92" s="98"/>
       <c r="AQ92" s="72"/>
       <c r="AR92" s="72"/>
-      <c r="AS92" s="101">
+      <c r="AS92" s="98">
         <v>9</v>
       </c>
-      <c r="AT92" s="101"/>
+      <c r="AT92" s="98"/>
       <c r="AU92" s="72"/>
       <c r="AV92" s="8"/>
       <c r="AW92" s="8"/>
@@ -8179,46 +8106,46 @@
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="18"/>
-      <c r="G94" s="98"/>
-      <c r="H94" s="99"/>
+      <c r="G94" s="99"/>
+      <c r="H94" s="100"/>
       <c r="I94" s="9"/>
-      <c r="J94" s="99"/>
-      <c r="K94" s="100"/>
-      <c r="L94" s="98"/>
-      <c r="M94" s="99"/>
+      <c r="J94" s="100"/>
+      <c r="K94" s="101"/>
+      <c r="L94" s="99"/>
+      <c r="M94" s="100"/>
       <c r="N94" s="9"/>
-      <c r="O94" s="99"/>
-      <c r="P94" s="100"/>
-      <c r="Q94" s="98"/>
-      <c r="R94" s="99"/>
+      <c r="O94" s="100"/>
+      <c r="P94" s="101"/>
+      <c r="Q94" s="99"/>
+      <c r="R94" s="100"/>
       <c r="S94" s="9"/>
-      <c r="T94" s="99"/>
-      <c r="U94" s="100"/>
-      <c r="V94" s="98"/>
-      <c r="W94" s="99"/>
+      <c r="T94" s="100"/>
+      <c r="U94" s="101"/>
+      <c r="V94" s="99"/>
+      <c r="W94" s="100"/>
       <c r="X94" s="9"/>
-      <c r="Y94" s="99"/>
-      <c r="Z94" s="100"/>
-      <c r="AA94" s="98"/>
-      <c r="AB94" s="99"/>
+      <c r="Y94" s="100"/>
+      <c r="Z94" s="101"/>
+      <c r="AA94" s="99"/>
+      <c r="AB94" s="100"/>
       <c r="AC94" s="9"/>
-      <c r="AD94" s="99"/>
-      <c r="AE94" s="100"/>
-      <c r="AF94" s="98"/>
-      <c r="AG94" s="99"/>
+      <c r="AD94" s="100"/>
+      <c r="AE94" s="101"/>
+      <c r="AF94" s="99"/>
+      <c r="AG94" s="100"/>
       <c r="AH94" s="9"/>
-      <c r="AI94" s="99"/>
-      <c r="AJ94" s="100"/>
-      <c r="AK94" s="98"/>
-      <c r="AL94" s="99"/>
+      <c r="AI94" s="100"/>
+      <c r="AJ94" s="101"/>
+      <c r="AK94" s="99"/>
+      <c r="AL94" s="100"/>
       <c r="AM94" s="9"/>
-      <c r="AN94" s="99"/>
-      <c r="AO94" s="100"/>
-      <c r="AP94" s="98"/>
-      <c r="AQ94" s="99"/>
+      <c r="AN94" s="100"/>
+      <c r="AO94" s="101"/>
+      <c r="AP94" s="99"/>
+      <c r="AQ94" s="100"/>
       <c r="AR94" s="9"/>
-      <c r="AS94" s="99"/>
-      <c r="AT94" s="100"/>
+      <c r="AS94" s="100"/>
+      <c r="AT94" s="101"/>
       <c r="AU94" s="21"/>
       <c r="AV94" s="8"/>
       <c r="AW94" s="8"/>
@@ -8908,64 +8835,64 @@
       <c r="D105" s="8"/>
       <c r="E105" s="8"/>
       <c r="F105" s="72"/>
-      <c r="G105" s="101">
+      <c r="G105" s="98">
         <v>1</v>
       </c>
-      <c r="H105" s="101"/>
+      <c r="H105" s="98"/>
       <c r="I105" s="72"/>
       <c r="J105" s="72"/>
-      <c r="K105" s="101">
+      <c r="K105" s="98">
         <v>2</v>
       </c>
-      <c r="L105" s="101"/>
+      <c r="L105" s="98"/>
       <c r="M105" s="72"/>
       <c r="N105" s="72"/>
       <c r="O105" s="72"/>
-      <c r="P105" s="101">
+      <c r="P105" s="98">
         <v>3</v>
       </c>
-      <c r="Q105" s="101"/>
+      <c r="Q105" s="98"/>
       <c r="R105" s="72"/>
       <c r="S105" s="72"/>
       <c r="T105" s="72"/>
-      <c r="U105" s="101">
+      <c r="U105" s="98">
         <v>4</v>
       </c>
-      <c r="V105" s="101"/>
+      <c r="V105" s="98"/>
       <c r="W105" s="72"/>
       <c r="X105" s="72"/>
       <c r="Y105" s="72"/>
-      <c r="Z105" s="101">
+      <c r="Z105" s="98">
         <v>5</v>
       </c>
-      <c r="AA105" s="101"/>
+      <c r="AA105" s="98"/>
       <c r="AB105" s="72"/>
       <c r="AC105" s="72"/>
       <c r="AD105" s="72"/>
-      <c r="AE105" s="101">
+      <c r="AE105" s="98">
         <v>6</v>
       </c>
-      <c r="AF105" s="101"/>
+      <c r="AF105" s="98"/>
       <c r="AG105" s="72"/>
       <c r="AH105" s="72"/>
       <c r="AI105" s="72"/>
-      <c r="AJ105" s="101">
+      <c r="AJ105" s="98">
         <v>7</v>
       </c>
-      <c r="AK105" s="101"/>
+      <c r="AK105" s="98"/>
       <c r="AL105" s="72"/>
       <c r="AM105" s="72"/>
       <c r="AN105" s="72"/>
-      <c r="AO105" s="101">
+      <c r="AO105" s="98">
         <v>8</v>
       </c>
-      <c r="AP105" s="101"/>
+      <c r="AP105" s="98"/>
       <c r="AQ105" s="72"/>
       <c r="AR105" s="72"/>
-      <c r="AS105" s="101">
+      <c r="AS105" s="98">
         <v>9</v>
       </c>
-      <c r="AT105" s="101"/>
+      <c r="AT105" s="98"/>
       <c r="AU105" s="72"/>
       <c r="AV105" s="8"/>
       <c r="AW105" s="8"/>
@@ -9060,46 +8987,46 @@
       </c>
       <c r="E107" s="8"/>
       <c r="F107" s="18"/>
-      <c r="G107" s="98"/>
-      <c r="H107" s="99"/>
+      <c r="G107" s="99"/>
+      <c r="H107" s="100"/>
       <c r="I107" s="9"/>
-      <c r="J107" s="99"/>
-      <c r="K107" s="100"/>
-      <c r="L107" s="98"/>
-      <c r="M107" s="99"/>
+      <c r="J107" s="100"/>
+      <c r="K107" s="101"/>
+      <c r="L107" s="99"/>
+      <c r="M107" s="100"/>
       <c r="N107" s="9"/>
-      <c r="O107" s="99"/>
-      <c r="P107" s="100"/>
-      <c r="Q107" s="98"/>
-      <c r="R107" s="99"/>
+      <c r="O107" s="100"/>
+      <c r="P107" s="101"/>
+      <c r="Q107" s="99"/>
+      <c r="R107" s="100"/>
       <c r="S107" s="9"/>
-      <c r="T107" s="99"/>
-      <c r="U107" s="100"/>
-      <c r="V107" s="98"/>
-      <c r="W107" s="99"/>
+      <c r="T107" s="100"/>
+      <c r="U107" s="101"/>
+      <c r="V107" s="99"/>
+      <c r="W107" s="100"/>
       <c r="X107" s="9"/>
-      <c r="Y107" s="99"/>
-      <c r="Z107" s="100"/>
-      <c r="AA107" s="98"/>
-      <c r="AB107" s="99"/>
+      <c r="Y107" s="100"/>
+      <c r="Z107" s="101"/>
+      <c r="AA107" s="99"/>
+      <c r="AB107" s="100"/>
       <c r="AC107" s="9"/>
-      <c r="AD107" s="99"/>
-      <c r="AE107" s="100"/>
-      <c r="AF107" s="98"/>
-      <c r="AG107" s="99"/>
+      <c r="AD107" s="100"/>
+      <c r="AE107" s="101"/>
+      <c r="AF107" s="99"/>
+      <c r="AG107" s="100"/>
       <c r="AH107" s="9"/>
-      <c r="AI107" s="99"/>
-      <c r="AJ107" s="100"/>
-      <c r="AK107" s="98"/>
-      <c r="AL107" s="99"/>
+      <c r="AI107" s="100"/>
+      <c r="AJ107" s="101"/>
+      <c r="AK107" s="99"/>
+      <c r="AL107" s="100"/>
       <c r="AM107" s="9"/>
-      <c r="AN107" s="99"/>
-      <c r="AO107" s="100"/>
-      <c r="AP107" s="98"/>
-      <c r="AQ107" s="99"/>
+      <c r="AN107" s="100"/>
+      <c r="AO107" s="101"/>
+      <c r="AP107" s="99"/>
+      <c r="AQ107" s="100"/>
       <c r="AR107" s="9"/>
-      <c r="AS107" s="99"/>
-      <c r="AT107" s="100"/>
+      <c r="AS107" s="100"/>
+      <c r="AT107" s="101"/>
       <c r="AU107" s="21"/>
       <c r="AV107" s="8"/>
       <c r="AW107" s="8"/>
@@ -9789,8 +9716,8 @@
       <c r="D118" s="15"/>
       <c r="E118" s="15"/>
       <c r="F118" s="9"/>
-      <c r="G118" s="98"/>
-      <c r="H118" s="99"/>
+      <c r="G118" s="99"/>
+      <c r="H118" s="100"/>
       <c r="I118" s="9"/>
       <c r="J118" s="9"/>
       <c r="K118" s="9"/>
@@ -9800,8 +9727,8 @@
       <c r="O118" s="9"/>
       <c r="P118" s="9"/>
       <c r="Q118" s="9"/>
-      <c r="R118" s="99"/>
-      <c r="S118" s="100"/>
+      <c r="R118" s="100"/>
+      <c r="S118" s="101"/>
       <c r="T118" s="9"/>
       <c r="U118" s="9"/>
       <c r="V118" s="9"/>
@@ -9816,8 +9743,8 @@
       <c r="AE118" s="9"/>
       <c r="AF118" s="9"/>
       <c r="AG118" s="9"/>
-      <c r="AH118" s="98"/>
-      <c r="AI118" s="99"/>
+      <c r="AH118" s="99"/>
+      <c r="AI118" s="100"/>
       <c r="AJ118" s="9"/>
       <c r="AK118" s="9"/>
       <c r="AL118" s="9"/>
@@ -9827,8 +9754,8 @@
       <c r="AP118" s="9"/>
       <c r="AQ118" s="9"/>
       <c r="AR118" s="9"/>
-      <c r="AS118" s="99"/>
-      <c r="AT118" s="100"/>
+      <c r="AS118" s="100"/>
+      <c r="AT118" s="101"/>
       <c r="AV118" s="9"/>
       <c r="AW118" s="9"/>
       <c r="AX118" s="9"/>
@@ -10241,64 +10168,64 @@
       <c r="D125" s="8"/>
       <c r="E125" s="8"/>
       <c r="F125" s="72"/>
-      <c r="G125" s="101">
+      <c r="G125" s="98">
         <v>1</v>
       </c>
-      <c r="H125" s="101"/>
+      <c r="H125" s="98"/>
       <c r="I125" s="72"/>
       <c r="J125" s="72"/>
-      <c r="K125" s="101">
+      <c r="K125" s="98">
         <v>2</v>
       </c>
-      <c r="L125" s="101"/>
+      <c r="L125" s="98"/>
       <c r="M125" s="72"/>
       <c r="N125" s="72"/>
       <c r="O125" s="72"/>
-      <c r="P125" s="101">
+      <c r="P125" s="98">
         <v>3</v>
       </c>
-      <c r="Q125" s="101"/>
+      <c r="Q125" s="98"/>
       <c r="R125" s="72"/>
       <c r="S125" s="72"/>
       <c r="T125" s="72"/>
-      <c r="U125" s="101">
+      <c r="U125" s="98">
         <v>4</v>
       </c>
-      <c r="V125" s="101"/>
+      <c r="V125" s="98"/>
       <c r="W125" s="72"/>
       <c r="X125" s="72"/>
       <c r="Y125" s="72"/>
-      <c r="Z125" s="101">
+      <c r="Z125" s="98">
         <v>5</v>
       </c>
-      <c r="AA125" s="101"/>
+      <c r="AA125" s="98"/>
       <c r="AB125" s="72"/>
       <c r="AC125" s="72"/>
       <c r="AD125" s="72"/>
-      <c r="AE125" s="101">
+      <c r="AE125" s="98">
         <v>6</v>
       </c>
-      <c r="AF125" s="101"/>
+      <c r="AF125" s="98"/>
       <c r="AG125" s="72"/>
       <c r="AH125" s="72"/>
       <c r="AI125" s="72"/>
-      <c r="AJ125" s="101">
+      <c r="AJ125" s="98">
         <v>7</v>
       </c>
-      <c r="AK125" s="101"/>
+      <c r="AK125" s="98"/>
       <c r="AL125" s="72"/>
       <c r="AM125" s="72"/>
       <c r="AN125" s="72"/>
-      <c r="AO125" s="101">
+      <c r="AO125" s="98">
         <v>8</v>
       </c>
-      <c r="AP125" s="101"/>
+      <c r="AP125" s="98"/>
       <c r="AQ125" s="72"/>
       <c r="AR125" s="72"/>
-      <c r="AS125" s="101">
+      <c r="AS125" s="98">
         <v>9</v>
       </c>
-      <c r="AT125" s="101"/>
+      <c r="AT125" s="98"/>
       <c r="AU125" s="72"/>
       <c r="AV125" s="8"/>
       <c r="AW125" s="8"/>
@@ -10393,46 +10320,46 @@
       </c>
       <c r="E127" s="8"/>
       <c r="F127" s="18"/>
-      <c r="G127" s="98"/>
-      <c r="H127" s="99"/>
+      <c r="G127" s="99"/>
+      <c r="H127" s="100"/>
       <c r="I127" s="9"/>
-      <c r="J127" s="99"/>
-      <c r="K127" s="100"/>
-      <c r="L127" s="98"/>
-      <c r="M127" s="99"/>
+      <c r="J127" s="100"/>
+      <c r="K127" s="101"/>
+      <c r="L127" s="99"/>
+      <c r="M127" s="100"/>
       <c r="N127" s="9"/>
-      <c r="O127" s="99"/>
-      <c r="P127" s="100"/>
-      <c r="Q127" s="98"/>
-      <c r="R127" s="99"/>
+      <c r="O127" s="100"/>
+      <c r="P127" s="101"/>
+      <c r="Q127" s="99"/>
+      <c r="R127" s="100"/>
       <c r="S127" s="9"/>
-      <c r="T127" s="99"/>
-      <c r="U127" s="100"/>
-      <c r="V127" s="98"/>
-      <c r="W127" s="99"/>
+      <c r="T127" s="100"/>
+      <c r="U127" s="101"/>
+      <c r="V127" s="99"/>
+      <c r="W127" s="100"/>
       <c r="X127" s="9"/>
-      <c r="Y127" s="99"/>
-      <c r="Z127" s="100"/>
-      <c r="AA127" s="98"/>
-      <c r="AB127" s="99"/>
+      <c r="Y127" s="100"/>
+      <c r="Z127" s="101"/>
+      <c r="AA127" s="99"/>
+      <c r="AB127" s="100"/>
       <c r="AC127" s="9"/>
-      <c r="AD127" s="99"/>
-      <c r="AE127" s="100"/>
-      <c r="AF127" s="98"/>
-      <c r="AG127" s="99"/>
+      <c r="AD127" s="100"/>
+      <c r="AE127" s="101"/>
+      <c r="AF127" s="99"/>
+      <c r="AG127" s="100"/>
       <c r="AH127" s="9"/>
-      <c r="AI127" s="99"/>
-      <c r="AJ127" s="100"/>
-      <c r="AK127" s="98"/>
-      <c r="AL127" s="99"/>
+      <c r="AI127" s="100"/>
+      <c r="AJ127" s="101"/>
+      <c r="AK127" s="99"/>
+      <c r="AL127" s="100"/>
       <c r="AM127" s="9"/>
-      <c r="AN127" s="99"/>
-      <c r="AO127" s="100"/>
-      <c r="AP127" s="98"/>
-      <c r="AQ127" s="99"/>
+      <c r="AN127" s="100"/>
+      <c r="AO127" s="101"/>
+      <c r="AP127" s="99"/>
+      <c r="AQ127" s="100"/>
       <c r="AR127" s="9"/>
-      <c r="AS127" s="99"/>
-      <c r="AT127" s="100"/>
+      <c r="AS127" s="100"/>
+      <c r="AT127" s="101"/>
       <c r="AU127" s="21"/>
       <c r="AV127" s="8"/>
       <c r="AW127" s="8"/>
@@ -11206,51 +11133,51 @@
       <c r="C139" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D139" s="98"/>
-      <c r="E139" s="99"/>
+      <c r="D139" s="99"/>
+      <c r="E139" s="100"/>
       <c r="F139" s="9"/>
-      <c r="G139" s="99"/>
-      <c r="H139" s="100"/>
-      <c r="I139" s="98"/>
-      <c r="J139" s="99"/>
+      <c r="G139" s="100"/>
+      <c r="H139" s="101"/>
+      <c r="I139" s="99"/>
+      <c r="J139" s="100"/>
       <c r="K139" s="9"/>
-      <c r="L139" s="99"/>
-      <c r="M139" s="100"/>
-      <c r="N139" s="98"/>
-      <c r="O139" s="99"/>
+      <c r="L139" s="100"/>
+      <c r="M139" s="101"/>
+      <c r="N139" s="99"/>
+      <c r="O139" s="100"/>
       <c r="P139" s="9"/>
-      <c r="Q139" s="99"/>
-      <c r="R139" s="100"/>
-      <c r="S139" s="98"/>
-      <c r="T139" s="99"/>
+      <c r="Q139" s="100"/>
+      <c r="R139" s="101"/>
+      <c r="S139" s="99"/>
+      <c r="T139" s="100"/>
       <c r="U139" s="9"/>
-      <c r="V139" s="99"/>
-      <c r="W139" s="100"/>
-      <c r="X139" s="98"/>
-      <c r="Y139" s="99"/>
+      <c r="V139" s="100"/>
+      <c r="W139" s="101"/>
+      <c r="X139" s="99"/>
+      <c r="Y139" s="100"/>
       <c r="Z139" s="9"/>
-      <c r="AA139" s="99"/>
-      <c r="AB139" s="100"/>
-      <c r="AC139" s="98"/>
-      <c r="AD139" s="99"/>
+      <c r="AA139" s="100"/>
+      <c r="AB139" s="101"/>
+      <c r="AC139" s="99"/>
+      <c r="AD139" s="100"/>
       <c r="AE139" s="9"/>
-      <c r="AF139" s="99"/>
-      <c r="AG139" s="100"/>
-      <c r="AH139" s="98"/>
-      <c r="AI139" s="99"/>
+      <c r="AF139" s="100"/>
+      <c r="AG139" s="101"/>
+      <c r="AH139" s="99"/>
+      <c r="AI139" s="100"/>
       <c r="AJ139" s="9"/>
-      <c r="AK139" s="99"/>
-      <c r="AL139" s="100"/>
-      <c r="AM139" s="98"/>
-      <c r="AN139" s="99"/>
+      <c r="AK139" s="100"/>
+      <c r="AL139" s="101"/>
+      <c r="AM139" s="99"/>
+      <c r="AN139" s="100"/>
       <c r="AO139" s="9"/>
-      <c r="AP139" s="99"/>
-      <c r="AQ139" s="100"/>
-      <c r="AR139" s="98"/>
-      <c r="AS139" s="99"/>
+      <c r="AP139" s="100"/>
+      <c r="AQ139" s="101"/>
+      <c r="AR139" s="99"/>
+      <c r="AS139" s="100"/>
       <c r="AT139" s="9"/>
-      <c r="AU139" s="99"/>
-      <c r="AV139" s="100"/>
+      <c r="AU139" s="100"/>
+      <c r="AV139" s="101"/>
       <c r="AW139" s="43"/>
       <c r="AX139" s="8"/>
       <c r="AY139" s="33"/>
@@ -12842,6 +12769,20 @@
     <mergeCell ref="AN101:AO102"/>
     <mergeCell ref="AP101:AQ102"/>
     <mergeCell ref="AS101:AT102"/>
+    <mergeCell ref="AD101:AE102"/>
+    <mergeCell ref="AF101:AG102"/>
+    <mergeCell ref="AI101:AJ102"/>
+    <mergeCell ref="AF138:AI138"/>
+    <mergeCell ref="AK138:AN138"/>
+    <mergeCell ref="AN134:AO135"/>
+    <mergeCell ref="AP134:AQ135"/>
+    <mergeCell ref="AS134:AT135"/>
+    <mergeCell ref="AP138:AS138"/>
+    <mergeCell ref="AE105:AF105"/>
+    <mergeCell ref="AJ105:AK105"/>
+    <mergeCell ref="Z125:AA125"/>
+    <mergeCell ref="AE125:AF125"/>
+    <mergeCell ref="AJ125:AK125"/>
     <mergeCell ref="D139:E140"/>
     <mergeCell ref="G139:H140"/>
     <mergeCell ref="I139:J140"/>
@@ -12851,13 +12792,8 @@
     <mergeCell ref="V101:W102"/>
     <mergeCell ref="Y101:Z102"/>
     <mergeCell ref="AA101:AB102"/>
-    <mergeCell ref="AD101:AE102"/>
-    <mergeCell ref="AF101:AG102"/>
-    <mergeCell ref="AI101:AJ102"/>
     <mergeCell ref="V138:Y138"/>
     <mergeCell ref="AA138:AD138"/>
-    <mergeCell ref="AF138:AI138"/>
-    <mergeCell ref="AK138:AN138"/>
     <mergeCell ref="D138:E138"/>
     <mergeCell ref="G138:J138"/>
     <mergeCell ref="L138:O138"/>
@@ -12868,9 +12804,9 @@
     <mergeCell ref="O101:P102"/>
     <mergeCell ref="Q101:R102"/>
     <mergeCell ref="T101:U102"/>
-    <mergeCell ref="V94:W95"/>
-    <mergeCell ref="Y94:Z95"/>
-    <mergeCell ref="AA94:AB95"/>
+    <mergeCell ref="Z105:AA105"/>
+    <mergeCell ref="G105:H105"/>
+    <mergeCell ref="K105:L105"/>
     <mergeCell ref="AI81:AJ82"/>
     <mergeCell ref="AK88:AL89"/>
     <mergeCell ref="AN88:AO89"/>
@@ -12892,6 +12828,11 @@
     <mergeCell ref="AN94:AO95"/>
     <mergeCell ref="AP94:AQ95"/>
     <mergeCell ref="AS94:AT95"/>
+    <mergeCell ref="V68:W69"/>
+    <mergeCell ref="Y68:Z69"/>
+    <mergeCell ref="AA68:AB69"/>
+    <mergeCell ref="AD68:AE69"/>
+    <mergeCell ref="AS68:AT69"/>
     <mergeCell ref="AD94:AE95"/>
     <mergeCell ref="AF94:AG95"/>
     <mergeCell ref="AI94:AJ95"/>
@@ -12901,15 +12842,21 @@
     <mergeCell ref="O88:P89"/>
     <mergeCell ref="Q88:R89"/>
     <mergeCell ref="T88:U89"/>
-    <mergeCell ref="V81:W82"/>
-    <mergeCell ref="Y81:Z82"/>
-    <mergeCell ref="AA81:AB82"/>
-    <mergeCell ref="AF68:AG69"/>
-    <mergeCell ref="AI68:AJ69"/>
-    <mergeCell ref="AK75:AL76"/>
-    <mergeCell ref="AN75:AO76"/>
-    <mergeCell ref="AP75:AQ76"/>
-    <mergeCell ref="AS75:AT76"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="K92:L92"/>
+    <mergeCell ref="P92:Q92"/>
+    <mergeCell ref="U92:V92"/>
+    <mergeCell ref="Z92:AA92"/>
+    <mergeCell ref="AE92:AF92"/>
+    <mergeCell ref="AJ92:AK92"/>
+    <mergeCell ref="V94:W95"/>
+    <mergeCell ref="Y94:Z95"/>
+    <mergeCell ref="AA94:AB95"/>
+    <mergeCell ref="P66:Q66"/>
+    <mergeCell ref="U66:V66"/>
+    <mergeCell ref="Z66:AA66"/>
+    <mergeCell ref="AE66:AF66"/>
+    <mergeCell ref="AJ66:AK66"/>
     <mergeCell ref="G81:H82"/>
     <mergeCell ref="J81:K82"/>
     <mergeCell ref="L81:M82"/>
@@ -12919,33 +12866,19 @@
     <mergeCell ref="V75:W76"/>
     <mergeCell ref="Y75:Z76"/>
     <mergeCell ref="AA75:AB76"/>
-    <mergeCell ref="AD75:AE76"/>
-    <mergeCell ref="AF75:AG76"/>
-    <mergeCell ref="AI75:AJ76"/>
-    <mergeCell ref="AK81:AL82"/>
-    <mergeCell ref="AN81:AO82"/>
-    <mergeCell ref="AP81:AQ82"/>
-    <mergeCell ref="AS81:AT82"/>
-    <mergeCell ref="AD81:AE82"/>
-    <mergeCell ref="AF81:AG82"/>
     <mergeCell ref="J75:K76"/>
     <mergeCell ref="L75:M76"/>
     <mergeCell ref="O75:P76"/>
     <mergeCell ref="Q75:R76"/>
     <mergeCell ref="T75:U76"/>
-    <mergeCell ref="V68:W69"/>
-    <mergeCell ref="Y68:Z69"/>
-    <mergeCell ref="AA68:AB69"/>
-    <mergeCell ref="AD68:AE69"/>
-    <mergeCell ref="AF55:AG56"/>
-    <mergeCell ref="AI55:AJ56"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="P66:Q66"/>
-    <mergeCell ref="U66:V66"/>
-    <mergeCell ref="Z66:AA66"/>
-    <mergeCell ref="AE66:AF66"/>
-    <mergeCell ref="AJ66:AK66"/>
+    <mergeCell ref="V81:W82"/>
+    <mergeCell ref="Y81:Z82"/>
+    <mergeCell ref="AA81:AB82"/>
+    <mergeCell ref="AF68:AG69"/>
+    <mergeCell ref="AI68:AJ69"/>
+    <mergeCell ref="V42:W43"/>
+    <mergeCell ref="Y42:Z43"/>
+    <mergeCell ref="AA42:AB43"/>
     <mergeCell ref="AK48:AL49"/>
     <mergeCell ref="AN48:AO49"/>
     <mergeCell ref="AP48:AQ49"/>
@@ -12967,18 +12900,6 @@
     <mergeCell ref="AP55:AQ56"/>
     <mergeCell ref="AS55:AT56"/>
     <mergeCell ref="V55:W56"/>
-    <mergeCell ref="Y55:Z56"/>
-    <mergeCell ref="AA55:AB56"/>
-    <mergeCell ref="AD55:AE56"/>
-    <mergeCell ref="G48:H49"/>
-    <mergeCell ref="J48:K49"/>
-    <mergeCell ref="L48:M49"/>
-    <mergeCell ref="O48:P49"/>
-    <mergeCell ref="Q48:R49"/>
-    <mergeCell ref="T48:U49"/>
-    <mergeCell ref="V42:W43"/>
-    <mergeCell ref="Y42:Z43"/>
-    <mergeCell ref="AA42:AB43"/>
     <mergeCell ref="AK35:AL36"/>
     <mergeCell ref="AN35:AO36"/>
     <mergeCell ref="AP35:AQ36"/>
@@ -13003,7 +12924,6 @@
     <mergeCell ref="AF42:AG43"/>
     <mergeCell ref="AI42:AJ43"/>
     <mergeCell ref="G35:H36"/>
-    <mergeCell ref="J35:K36"/>
     <mergeCell ref="L35:M36"/>
     <mergeCell ref="O35:P36"/>
     <mergeCell ref="Q35:R36"/>
@@ -13025,26 +12945,45 @@
     <mergeCell ref="AF10:AG11"/>
     <mergeCell ref="AJ79:AK79"/>
     <mergeCell ref="AO79:AP79"/>
-    <mergeCell ref="G92:H92"/>
-    <mergeCell ref="K92:L92"/>
-    <mergeCell ref="P92:Q92"/>
-    <mergeCell ref="U92:V92"/>
-    <mergeCell ref="Z92:AA92"/>
-    <mergeCell ref="AE92:AF92"/>
-    <mergeCell ref="AJ92:AK92"/>
-    <mergeCell ref="AO92:AP92"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="K79:L79"/>
-    <mergeCell ref="P79:Q79"/>
-    <mergeCell ref="U79:V79"/>
-    <mergeCell ref="Z79:AA79"/>
-    <mergeCell ref="AE79:AF79"/>
-    <mergeCell ref="AJ46:AK46"/>
-    <mergeCell ref="AO46:AP46"/>
     <mergeCell ref="V16:W17"/>
     <mergeCell ref="AF16:AG17"/>
     <mergeCell ref="AI16:AJ17"/>
     <mergeCell ref="AK16:AL17"/>
+    <mergeCell ref="T10:U11"/>
+    <mergeCell ref="V10:W11"/>
+    <mergeCell ref="Y10:Z11"/>
+    <mergeCell ref="AA10:AB11"/>
+    <mergeCell ref="AD10:AE11"/>
+    <mergeCell ref="T16:U17"/>
+    <mergeCell ref="AN16:AO17"/>
+    <mergeCell ref="AN23:AO24"/>
+    <mergeCell ref="AP23:AQ24"/>
+    <mergeCell ref="AO14:AP14"/>
+    <mergeCell ref="J35:K36"/>
+    <mergeCell ref="AJ46:AK46"/>
+    <mergeCell ref="AO46:AP46"/>
+    <mergeCell ref="AO66:AP66"/>
+    <mergeCell ref="AN68:AO69"/>
+    <mergeCell ref="AP68:AQ69"/>
+    <mergeCell ref="G62:H63"/>
+    <mergeCell ref="R62:S63"/>
+    <mergeCell ref="AH62:AI63"/>
+    <mergeCell ref="G59:H60"/>
+    <mergeCell ref="R59:S60"/>
+    <mergeCell ref="AH59:AI60"/>
+    <mergeCell ref="G48:H49"/>
+    <mergeCell ref="J48:K49"/>
+    <mergeCell ref="L48:M49"/>
+    <mergeCell ref="O48:P49"/>
+    <mergeCell ref="Q48:R49"/>
+    <mergeCell ref="T48:U49"/>
+    <mergeCell ref="Y55:Z56"/>
+    <mergeCell ref="AA55:AB56"/>
+    <mergeCell ref="AD55:AE56"/>
+    <mergeCell ref="AF55:AG56"/>
+    <mergeCell ref="AI55:AJ56"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="K66:L66"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="Z1:AA1"/>
@@ -13093,11 +13032,6 @@
     <mergeCell ref="BA73:BB76"/>
     <mergeCell ref="BD16:BE24"/>
     <mergeCell ref="BA21:BB24"/>
-    <mergeCell ref="T10:U11"/>
-    <mergeCell ref="V10:W11"/>
-    <mergeCell ref="Y10:Z11"/>
-    <mergeCell ref="AA10:AB11"/>
-    <mergeCell ref="AD10:AE11"/>
     <mergeCell ref="AA3:AB4"/>
     <mergeCell ref="AD3:AE4"/>
     <mergeCell ref="AF3:AG4"/>
@@ -13108,14 +13042,10 @@
     <mergeCell ref="AD16:AE17"/>
     <mergeCell ref="AJ10:AK11"/>
     <mergeCell ref="AI23:AJ24"/>
-    <mergeCell ref="T16:U17"/>
     <mergeCell ref="AK23:AL24"/>
     <mergeCell ref="AA23:AB24"/>
     <mergeCell ref="AD23:AE24"/>
     <mergeCell ref="AF23:AG24"/>
-    <mergeCell ref="AN134:AO135"/>
-    <mergeCell ref="AP134:AQ135"/>
-    <mergeCell ref="AS134:AT135"/>
     <mergeCell ref="BA35:BB38"/>
     <mergeCell ref="BD35:BE43"/>
     <mergeCell ref="BA40:BB43"/>
@@ -13125,15 +13055,7 @@
     <mergeCell ref="BA3:BB6"/>
     <mergeCell ref="BA16:BB19"/>
     <mergeCell ref="AS33:AT33"/>
-    <mergeCell ref="AN16:AO17"/>
-    <mergeCell ref="AN23:AO24"/>
-    <mergeCell ref="AP23:AQ24"/>
     <mergeCell ref="AS23:AT24"/>
-    <mergeCell ref="AO66:AP66"/>
-    <mergeCell ref="AN68:AO69"/>
-    <mergeCell ref="AP68:AQ69"/>
-    <mergeCell ref="AS68:AT69"/>
-    <mergeCell ref="AO14:AP14"/>
     <mergeCell ref="AS14:AT14"/>
     <mergeCell ref="AS46:AT46"/>
     <mergeCell ref="AS66:AT66"/>
@@ -13144,7 +13066,16 @@
     <mergeCell ref="AN127:AO128"/>
     <mergeCell ref="AP127:AQ128"/>
     <mergeCell ref="AS127:AT128"/>
-    <mergeCell ref="AP138:AS138"/>
+    <mergeCell ref="AS62:AT63"/>
+    <mergeCell ref="AO105:AP105"/>
+    <mergeCell ref="AO125:AP125"/>
+    <mergeCell ref="AO92:AP92"/>
+    <mergeCell ref="AN75:AO76"/>
+    <mergeCell ref="AP75:AQ76"/>
+    <mergeCell ref="AS75:AT76"/>
+    <mergeCell ref="AN81:AO82"/>
+    <mergeCell ref="AP81:AQ82"/>
+    <mergeCell ref="AS81:AT82"/>
     <mergeCell ref="BG15:BJ15"/>
     <mergeCell ref="BG16:BJ16"/>
     <mergeCell ref="BG17:BG18"/>
@@ -13211,8 +13142,6 @@
     <mergeCell ref="BH86:BJ87"/>
     <mergeCell ref="BG88:BG89"/>
     <mergeCell ref="BH88:BJ89"/>
-    <mergeCell ref="BG134:BG135"/>
-    <mergeCell ref="BH134:BJ135"/>
     <mergeCell ref="BG97:BG98"/>
     <mergeCell ref="BH97:BJ98"/>
     <mergeCell ref="BG99:BG100"/>
@@ -13253,19 +13182,6 @@
     <mergeCell ref="BG108:BG109"/>
     <mergeCell ref="BH108:BJ109"/>
     <mergeCell ref="BG110:BG111"/>
-    <mergeCell ref="G62:H63"/>
-    <mergeCell ref="R62:S63"/>
-    <mergeCell ref="AH62:AI63"/>
-    <mergeCell ref="AS62:AT63"/>
-    <mergeCell ref="G59:H60"/>
-    <mergeCell ref="R59:S60"/>
-    <mergeCell ref="AH59:AI60"/>
-    <mergeCell ref="Z105:AA105"/>
-    <mergeCell ref="AE105:AF105"/>
-    <mergeCell ref="AJ105:AK105"/>
-    <mergeCell ref="AO105:AP105"/>
-    <mergeCell ref="G105:H105"/>
-    <mergeCell ref="K105:L105"/>
     <mergeCell ref="P105:Q105"/>
     <mergeCell ref="U105:V105"/>
     <mergeCell ref="AS105:AT105"/>
@@ -13277,6 +13193,19 @@
     <mergeCell ref="T68:U69"/>
     <mergeCell ref="AK68:AL69"/>
     <mergeCell ref="G75:H76"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="K79:L79"/>
+    <mergeCell ref="P79:Q79"/>
+    <mergeCell ref="U79:V79"/>
+    <mergeCell ref="Z79:AA79"/>
+    <mergeCell ref="AE79:AF79"/>
+    <mergeCell ref="AK75:AL76"/>
+    <mergeCell ref="AD75:AE76"/>
+    <mergeCell ref="AF75:AG76"/>
+    <mergeCell ref="AI75:AJ76"/>
+    <mergeCell ref="AK81:AL82"/>
+    <mergeCell ref="AD81:AE82"/>
+    <mergeCell ref="AF81:AG82"/>
     <mergeCell ref="G107:H108"/>
     <mergeCell ref="J107:K108"/>
     <mergeCell ref="L107:M108"/>
@@ -13318,10 +13247,6 @@
     <mergeCell ref="R118:S119"/>
     <mergeCell ref="AH118:AI119"/>
     <mergeCell ref="AS118:AT119"/>
-    <mergeCell ref="Z125:AA125"/>
-    <mergeCell ref="AE125:AF125"/>
-    <mergeCell ref="AJ125:AK125"/>
-    <mergeCell ref="AO125:AP125"/>
     <mergeCell ref="G125:H125"/>
     <mergeCell ref="K125:L125"/>
     <mergeCell ref="P125:Q125"/>
@@ -13350,6 +13275,8 @@
     <mergeCell ref="BA132:BB135"/>
     <mergeCell ref="BG132:BG133"/>
     <mergeCell ref="BH132:BJ133"/>
+    <mergeCell ref="BG134:BG135"/>
+    <mergeCell ref="BH134:BJ135"/>
     <mergeCell ref="Q134:R135"/>
     <mergeCell ref="T134:U135"/>
     <mergeCell ref="V134:W135"/>

</xml_diff>